<commit_message>
polished the parser for csv/excel as well as the course model and the csv/excel generator, as well as the API endpoints
</commit_message>
<xml_diff>
--- a/backend/src/uploads/files/professor-courselist (1).xlsx
+++ b/backend/src/uploads/files/professor-courselist (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\MSCS\TA\CS Project\GAS\Input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jasontran2048\UTD-Projects\Senior\S25\grader-assignment-system\backend\src\uploads\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{2A9F2A12-FCC7-43C0-B85C-E37F80838E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{679D8369-0546-4465-8AE3-F9BA844F4BB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895AA256-662A-4CDC-A169-AC6413C7DB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2670" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Professor Name</t>
   </si>
@@ -63,16 +63,70 @@
   </si>
   <si>
     <t>Keywords</t>
+  </si>
+  <si>
+    <t>Prof. Smith</t>
+  </si>
+  <si>
+    <t>Prof. Cole</t>
+  </si>
+  <si>
+    <t>John.Cole@utdallas.edu </t>
+  </si>
+  <si>
+    <t>Jason.Smith1@utdallas.edu</t>
+  </si>
+  <si>
+    <t>"001"</t>
+  </si>
+  <si>
+    <t>Computer Science II</t>
+  </si>
+  <si>
+    <t>Computer Architecture</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>jde200000</t>
+  </si>
+  <si>
+    <t>Ron Doe</t>
+  </si>
+  <si>
+    <t>rde200001</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF151515"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,14 +155,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,24 +445,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +492,69 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>2337</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2340</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="mailto:John.Cole@utdallas.edu" xr:uid="{15CD881E-1CE3-4C6F-8A2A-35BCDC939C93}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>